<commit_message>
Edited some css for about us
</commit_message>
<xml_diff>
--- a/backend/data/queries.xlsx
+++ b/backend/data/queries.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
   <si>
     <t>First Name</t>
   </si>
@@ -35,6 +35,24 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Gopal</t>
+  </si>
+  <si>
+    <t>Goyal</t>
+  </si>
+  <si>
+    <t>goyal11.gopal@gmail.com</t>
+  </si>
+  <si>
+    <t>09462976187</t>
+  </si>
+  <si>
+    <t>wassup</t>
+  </si>
+  <si>
+    <t>helloooo</t>
   </si>
 </sst>
 </file>
@@ -70,9 +88,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,52 +395,188 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.005" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.005" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.005" style="1" customWidth="1"/>
-    <col min="5" max="6" width="40.005" style="1" customWidth="1"/>
+    <col min="1" max="2" width="15.005" customWidth="1"/>
+    <col min="3" max="3" width="25.005" customWidth="1"/>
+    <col min="4" max="4" width="15.005" customWidth="1"/>
+    <col min="5" max="6" width="40.005" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>